<commit_message>
started on jump mechanic
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Personal project\Civilization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35D5D50-F8DB-446A-9712-5D6DE5E76253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8622FA09-DCCB-47C3-BBFE-5AC268767E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="5145" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Day</t>
   </si>
@@ -60,6 +58,12 @@
   </si>
   <si>
     <t>Set up Git repository</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Started working on character controls</t>
   </si>
 </sst>
 </file>
@@ -395,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -452,6 +456,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45769</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Work on jump mechanic
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8622FA09-DCCB-47C3-BBFE-5AC268767E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A3AA6F-7404-4947-A754-B41492222396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Day</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Started working on character controls</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Started on jump</t>
   </si>
 </sst>
 </file>
@@ -113,15 +119,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -399,23 +406,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -456,7 +463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -474,6 +481,26 @@
       </c>
       <c r="F3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45770</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on camera and character slerping
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB0EC07-FD75-4108-9B32-A01B15C67EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91984F54-846D-444F-930F-F5366B408713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Day</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Working on jump mechanic</t>
+  </si>
+  <si>
+    <t>Working on jump mechanic, camera movement</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,7 +464,7 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="E2" s="3">
-        <f>D2-C2</f>
+        <f t="shared" ref="E2:E5" si="0">D2-C2</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F2" t="s">
@@ -482,7 +485,8 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E3" s="3">
-        <v>8.3333333333333329E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -502,7 +506,8 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="E4" s="3">
-        <v>2.0833333333333332E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -522,10 +527,32 @@
         <v>0.5625</v>
       </c>
       <c r="E5" s="3">
-        <v>2.0833333333333332E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4">
+        <v>45771</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6-C6</f>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suffering on character controler
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91984F54-846D-444F-930F-F5366B408713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2806F62-7CBA-43AC-876B-7C487B4115DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Day</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Working on jump mechanic, camera movement</t>
+  </si>
+  <si>
+    <t>Suffering on camera movement</t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,23 +417,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="6" width="45.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -471,7 +474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -492,7 +495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -513,7 +516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -534,7 +537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -553,6 +556,27 @@
       </c>
       <c r="F6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>45773</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E7" s="3">
+        <f>D7-C7</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed camera movement, working on ADS
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2806F62-7CBA-43AC-876B-7C487B4115DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFD7A21-92E9-4AE5-A1E2-5AEC77104612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Day</t>
   </si>
@@ -82,13 +82,25 @@
   </si>
   <si>
     <t>Suffering on camera movement</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Suffering on camera movement and character rotation, working on zoom</t>
+  </si>
+  <si>
+    <t>Total time spent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +112,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,12 +149,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -417,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +449,12 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" customWidth="1"/>
+    <col min="6" max="6" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +473,15 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="5">
+        <f>SUM(E:E)</f>
+        <v>0.4340277777777779</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -474,7 +502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -495,7 +523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -516,7 +544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -537,7 +565,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -558,7 +586,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -579,7 +607,29 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
+        <v>45774</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" s="3">
+        <f>D8-C8</f>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added camera collision with obstacles
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14BF001-65E2-413E-AFFE-2015A40E0092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714E0724-D6C2-470B-9991-42C342496CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Day</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Working on movement</t>
+  </si>
+  <si>
+    <t>Working on camera colision and movement</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -442,25 +445,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="6" width="66.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,10 +487,10 @@
       </c>
       <c r="I1" s="5">
         <f>SUM(E:E)</f>
-        <v>0.51736111111111116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.56597222222222232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -508,7 +511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -529,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -550,7 +553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -571,7 +574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -592,7 +595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -613,7 +616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -634,7 +637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -653,6 +656,27 @@
       </c>
       <c r="F9" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>45778</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="E10" s="3">
+        <f>D10-C10</f>
+        <v>4.861111111111116E-2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on crosshair and smoke power
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714E0724-D6C2-470B-9991-42C342496CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019C650D-3A00-4D62-B6B1-AC64954D3626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Day</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Working on camera colision and movement</t>
+  </si>
+  <si>
+    <t>Figuring out crosshair logic</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,25 +448,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="66.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,10 +490,10 @@
       </c>
       <c r="I1" s="5">
         <f>SUM(E:E)</f>
-        <v>0.56597222222222232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.64930555555555558</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -511,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -532,7 +535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -553,7 +556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -574,7 +577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -595,7 +598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -616,7 +619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -637,7 +640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -658,7 +661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -677,6 +680,27 @@
       </c>
       <c r="F10" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4">
+        <v>45782</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="E11" s="3">
+        <f>D11-C11</f>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on shooting and smoke dash
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019C650D-3A00-4D62-B6B1-AC64954D3626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C045FAF-6146-4AF1-AFE8-A9458B2D07BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Day</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Figuring out crosshair logic</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Trying to figure out shooting</t>
+  </si>
+  <si>
+    <t>Working on smoke dash</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -448,25 +457,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="6" width="66.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,10 +499,10 @@
       </c>
       <c r="I1" s="5">
         <f>SUM(E:E)</f>
-        <v>0.64930555555555558</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.94097222222222232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -514,7 +523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -535,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -556,7 +565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -577,7 +586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -591,14 +600,14 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E6" s="3">
-        <f>D6-C6</f>
+        <f t="shared" ref="E6:E13" si="1">D6-C6</f>
         <v>7.2916666666666741E-2</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -612,14 +621,14 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="E7" s="3">
-        <f>D7-C7</f>
+        <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -633,14 +642,14 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E8" s="3">
-        <f>D8-C8</f>
+        <f t="shared" si="1"/>
         <v>0.16666666666666674</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -654,14 +663,14 @@
         <v>0.4375</v>
       </c>
       <c r="E9" s="3">
-        <f>D9-C9</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333315E-2</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -675,14 +684,14 @@
         <v>0.84027777777777779</v>
       </c>
       <c r="E10" s="3">
-        <f>D10-C10</f>
+        <f t="shared" si="1"/>
         <v>4.861111111111116E-2</v>
       </c>
       <c r="F10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -696,11 +705,53 @@
         <v>0.4375</v>
       </c>
       <c r="E11" s="3">
-        <f>D11-C11</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333315E-2</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4">
+        <v>45786</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333337</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4">
+        <v>45788</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shooting and smoke dash
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAE2024-2025\2024-2025\Platform Development 2\Final_Assignment\Infamous_Second_Son\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C045FAF-6146-4AF1-AFE8-A9458B2D07BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16567E8-D50F-4773-9534-3CFFE40D4079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Day</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Working on smoke dash</t>
+  </si>
+  <si>
+    <t>Working on shooting &amp; smoke dash</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,25 +460,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="66.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,10 +502,10 @@
       </c>
       <c r="I1" s="5">
         <f>SUM(E:E)</f>
-        <v>0.94097222222222232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0243055555555556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -523,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -544,7 +547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -565,7 +568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -586,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -600,14 +603,14 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ref="E6:E13" si="1">D6-C6</f>
+        <f t="shared" ref="E6:E14" si="1">D6-C6</f>
         <v>7.2916666666666741E-2</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -628,7 +631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -649,7 +652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -670,7 +673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -691,7 +694,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -712,7 +715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -733,7 +736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -752,6 +755,27 @@
       </c>
       <c r="F13" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45789</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>